<commit_message>
add annotation for pricing data of trip booking on azure
</commit_message>
<xml_diff>
--- a/perf-cost/6200.trip-booking/azure/2024/pricing-6200.trip-booking.xlsx
+++ b/perf-cost/6200.trip-booking/azure/2024/pricing-6200.trip-booking.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Chart Title: </t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">6200-trip-booking-python-3-8-6d2d1d6a, Function Execution Units (Sum), 6200-trip-booking-python-3-8-6d2d1d6a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">warm invocations</t>
   </si>
 </sst>
 </file>
@@ -135,7 +138,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -145,6 +148,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -225,13 +232,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.98"/>
@@ -386,6 +393,9 @@
       </c>
       <c r="C20" s="2" t="n">
         <v>23657472</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>